<commit_message>
update excel progress, mo mandi, mo ashar
</commit_message>
<xml_diff>
--- a/docs/skripsi/Progress.xlsx
+++ b/docs/skripsi/Progress.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfauzanzulkarnaen/Documents/Project Skripsi/skripsi-yolov8/docs/skripsi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069C73D5-17DF-1849-A6BB-D0F99BF5FB14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4D17C5-E49B-3E43-A441-24C38409B92A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="20520" xr2:uid="{A05E2602-9300-1745-9CF0-C349C3E8FD48}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="2" r:id="rId1"/>
+    <sheet name="Note" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>bab 3 tulis identifikasi masalah</t>
   </si>
@@ -70,9 +71,6 @@
   </si>
   <si>
     <t>Pindahin identifikasi masalah di bab 3 ke latar belakang, karena harusnya di identifikasi masalah itu isinya tentang "struggle" pada penelitian, bukan data dan pengenalan kayak yang tertulis di v3</t>
-  </si>
-  <si>
-    <t>coba baca lagi skripsinya secara keseluruhan supaya tahu dimana penambahan yang pas, tapi untuk sekarang yang jelas di bab 2 perlu penambahan studi literatur</t>
   </si>
   <si>
     <t>Perubahan batasan masalah karena ga jadi buat API dan antarmuka</t>
@@ -99,11 +97,57 @@
   <si>
     <t>masih belum ada gambaran, belum review skripsi lain juga, masih nunggu proses dari PR yang diatas atas-nya</t>
   </si>
+  <si>
+    <t xml:space="preserve">coba baca lagi skripsinya secara keseluruhan supaya tahu dimana penambahan yang pas, tapi untuk sekarang yang jelas di bab 2 perlu penambahan studi literatur
+Bahan :
+1. CNN(udah), mungkin kita perpanjang aja lagi ya)
+2. Darknet
+3. Pytorch
+</t>
+  </si>
+  <si>
+    <t>To search</t>
+  </si>
+  <si>
+    <t>K means in CNN or YOLO or Deep Learning</t>
+  </si>
+  <si>
+    <t>What is CUDA and what is alternative for it</t>
+  </si>
+  <si>
+    <t>Compare CUDA and it alternatives or without CUDA</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Untuk sekarang progress di jeda dulu, darknet sama pytorch masih belum ada progress
+Tapi untuk CNN, YOLO sama Cuda udah ada jurnal tambahan, tinggal dicantumin aja lagi
+Mo balek, mandi, ashar dulu, mungkin malam lanjut</t>
+  </si>
+  <si>
+    <t>Pytorch (All information and journal)</t>
+  </si>
+  <si>
+    <t>Darknet (All information and journal)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -198,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -229,6 +273,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECB9053-5FF2-7044-9533-828A89616F7E}">
   <dimension ref="B2:E26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,7 +647,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>13</v>
@@ -615,7 +671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" ht="187" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -623,7 +679,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>10</v>
@@ -637,7 +693,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>7</v>
@@ -651,7 +707,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>7</v>
@@ -665,7 +721,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>1</v>
@@ -679,10 +735,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="51" x14ac:dyDescent="0.2">
@@ -693,7 +749,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>1</v>
@@ -707,10 +763,10 @@
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="85" x14ac:dyDescent="0.2">
@@ -721,13 +777,41 @@
         <v>0</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
     </row>
   </sheetData>
@@ -749,4 +833,51 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6442856-5F95-2C47-8D55-0ABD5674E0FC}">
+  <dimension ref="B3:E4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="137" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13">
+        <v>45388</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.7104166666666667</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add sheet 'progrgess 2'  to progress and add 'difficulty' to progress
</commit_message>
<xml_diff>
--- a/docs/skripsi/Progress.xlsx
+++ b/docs/skripsi/Progress.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfauzanzulkarnaen/Documents/Project Skripsi/skripsi-yolov8/docs/skripsi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BCA2DF-BDBF-5F48-B87F-15712E43CE28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB30197B-793F-5147-B1E8-F6931F98081A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="20520" xr2:uid="{A05E2602-9300-1745-9CF0-C349C3E8FD48}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="20520" activeTab="1" xr2:uid="{A05E2602-9300-1745-9CF0-C349C3E8FD48}"/>
   </bookViews>
   <sheets>
-    <sheet name="Progress" sheetId="2" r:id="rId1"/>
-    <sheet name="Note" sheetId="3" r:id="rId2"/>
-    <sheet name="Pytorch" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
+    <sheet name="Progress 1" sheetId="2" r:id="rId1"/>
+    <sheet name="Progress 2" sheetId="7" r:id="rId2"/>
+    <sheet name="Note" sheetId="3" r:id="rId3"/>
+    <sheet name="Pytorch" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="123">
   <si>
     <t>bab 3 tulis identifikasi masalah</t>
   </si>
@@ -367,6 +368,93 @@
   </si>
   <si>
     <t>The main steps of face detection technology involve finding the area in an image where a face or faces are. The main challenges in face detection are occlusion, illuminations, and complex background. A wide variety of algorithms have been proposed to combat these challenges. Basically, the available algorithms are divided mainly on two parts: feature-based and image-based approaches. While feature-based approaches find features (image edges, corners, and other structures well localized in two dimensions), image-based approaches depend largely on image scanning, which is based on window or sub-frames.</t>
+  </si>
+  <si>
+    <t>Keterangan Gambar</t>
+  </si>
+  <si>
+    <t>Keterangan Tabel</t>
+  </si>
+  <si>
+    <t>Kalimat kesimpulan di paragraf terakhir pada latar belakang</t>
+  </si>
+  <si>
+    <t>Perumusan masalah jika Menyinggung efektifitas dan efesiensi sertakan hasil pengukuran indikator tersebut di bab 4</t>
+  </si>
+  <si>
+    <t>Jika menyinggung keakuratan maka harus ada pembanding</t>
+  </si>
+  <si>
+    <t>Saran permasalahan dijadikan 3 point, dan 1 penekanan 2 nya pendukung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batasan masalah tidak perlu tertulis alasan, cukup menekankan batasan sesuai area penelitian. </t>
+  </si>
+  <si>
+    <t>Manfaat dijadikan bagi peneliti, pendidikan dan masyarakat</t>
+  </si>
+  <si>
+    <t>⁠Tabel penelitian terdahulu ditambahkan 3 kolom metode, keterkaitan penelitian dan pembaharuan</t>
+  </si>
+  <si>
+    <t>Bab 3 penjelasan kerangka penelitian berkaitan dengan penelitian dirisendiri bukan penjelasan umum</t>
+  </si>
+  <si>
+    <t>Penambahan Keterangan gambar dan sitasi</t>
+  </si>
+  <si>
+    <t>Penambahan Keterangan tabel</t>
+  </si>
+  <si>
+    <t>Pembuatan daftar tabel</t>
+  </si>
+  <si>
+    <t>Pembuatan daftar gambar</t>
+  </si>
+  <si>
+    <t>Buat daftar tabel</t>
+  </si>
+  <si>
+    <t>Merubah/menambah paragraf terakhir</t>
+  </si>
+  <si>
+    <t>===Questioanble at the best===</t>
+  </si>
+  <si>
+    <t>Waiting Hasil Training</t>
+  </si>
+  <si>
+    <t>Permasalahan itu yang mana?</t>
+  </si>
+  <si>
+    <t>Hapus alasan</t>
+  </si>
+  <si>
+    <t>Hapus manfaat bagi perkembangan teknologi dan tambah bagi pendidikan dan masyarakat</t>
+  </si>
+  <si>
+    <t>Duhhh, baca ulang dan tambahkan cari tahu metode, keterkaitan dan pembaruan</t>
+  </si>
+  <si>
+    <t>Ini nih gimana sih</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>WHATT????</t>
+  </si>
+  <si>
+    <t>EASY</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>HARD</t>
   </si>
 </sst>
 </file>
@@ -476,7 +564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -526,11 +614,135 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -563,6 +775,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF54BBFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -975,7 +1192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECB9053-5FF2-7044-9533-828A89616F7E}">
   <dimension ref="B2:E26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1171,13 +1388,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E11">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NOT YET">
+    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="NOT YET">
       <formula>NOT(ISERROR(SEARCH("NOT YET",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="ON PROGRESS">
+    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="ON PROGRESS">
       <formula>NOT(ISERROR(SEARCH("ON PROGRESS",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1192,6 +1409,281 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D64342-63FD-6945-A4D1-ADCC0106C171}">
+  <dimension ref="B2:F26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="39" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="51" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="2">
+        <v>7</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="2">
+        <v>9</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="22">
+        <v>10</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="22">
+        <v>11</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="22">
+        <v>12</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F3:F14">
+    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="NOT YET">
+      <formula>NOT(ISERROR(SEARCH("NOT YET",F3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="ON PROGRESS">
+      <formula>NOT(ISERROR(SEARCH("ON PROGRESS",F3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",F3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E14">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="EASY">
+      <formula>NOT(ISERROR(SEARCH("EASY",E3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="HARD">
+      <formula>NOT(ISERROR(SEARCH("HARD",E3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F14" xr:uid="{F3C3F2A3-C474-D04C-91EB-021D5BB25D98}">
+      <formula1>"DONE,ON PROGRESS,NOT YET"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E14" xr:uid="{4AA611BC-D7B5-FF4B-B9D9-783561503493}">
+      <formula1>"EASY,MEDIUM,HARD,WHATT????"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6442856-5F95-2C47-8D55-0ABD5674E0FC}">
   <dimension ref="B3:E5"/>
   <sheetViews>
@@ -1247,7 +1739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC091DCD-8BEB-5F43-A16C-3C3A53E95F29}">
   <dimension ref="B2:G192"/>
   <sheetViews>
@@ -2237,7 +2729,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6752C4-E658-D941-B38E-B79487B40535}">
   <dimension ref="B2:D11"/>
   <sheetViews>

</xml_diff>

<commit_message>
perbaiki typo di progress 2
</commit_message>
<xml_diff>
--- a/docs/skripsi/Progress.xlsx
+++ b/docs/skripsi/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfauzanzulkarnaen/Documents/Project Skripsi/skripsi-yolov8/docs/skripsi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB30197B-793F-5147-B1E8-F6931F98081A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F34AF04-C636-5844-9099-ED71C28D780E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="20520" activeTab="1" xr2:uid="{A05E2602-9300-1745-9CF0-C349C3E8FD48}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="124">
   <si>
     <t>bab 3 tulis identifikasi masalah</t>
   </si>
@@ -433,9 +433,6 @@
     <t>Hapus manfaat bagi perkembangan teknologi dan tambah bagi pendidikan dan masyarakat</t>
   </si>
   <si>
-    <t>Duhhh, baca ulang dan tambahkan cari tahu metode, keterkaitan dan pembaruan</t>
-  </si>
-  <si>
     <t>Ini nih gimana sih</t>
   </si>
   <si>
@@ -455,6 +452,12 @@
   </si>
   <si>
     <t>HARD</t>
+  </si>
+  <si>
+    <t>ON PROGRESS</t>
+  </si>
+  <si>
+    <t>Duhhh, baca ulang, cari tahu  dan tambahkan tentang metode, keterkaitan dan pembaruan</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1416,7 @@
   <dimension ref="B2:F26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1435,10 +1438,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="51" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1452,7 +1455,7 @@
         <v>104</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>7</v>
@@ -1469,7 +1472,7 @@
         <v>105</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>7</v>
@@ -1486,10 +1489,10 @@
         <v>109</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1503,7 +1506,7 @@
         <v>110</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>1</v>
@@ -1520,7 +1523,7 @@
         <v>111</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>1</v>
@@ -1537,7 +1540,7 @@
         <v>112</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>1</v>
@@ -1554,10 +1557,10 @@
         <v>113</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1571,10 +1574,10 @@
         <v>114</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1585,13 +1588,13 @@
         <v>102</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="E11" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1602,10 +1605,10 @@
         <v>103</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>1</v>
@@ -1622,10 +1625,10 @@
         <v>108</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1639,10 +1642,10 @@
         <v>108</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.2">
@@ -1744,8 +1747,8 @@
   <dimension ref="B2:G192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add tabel list jurnal referensi dan link pada sheet progress 2
</commit_message>
<xml_diff>
--- a/docs/skripsi/Progress.xlsx
+++ b/docs/skripsi/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfauzanzulkarnaen/Documents/Project Skripsi/skripsi-yolov8/docs/skripsi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F34AF04-C636-5844-9099-ED71C28D780E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BB4DEB-4F5E-8E45-8A11-8B01EBB125BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="20520" activeTab="1" xr2:uid="{A05E2602-9300-1745-9CF0-C349C3E8FD48}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="136">
   <si>
     <t>bab 3 tulis identifikasi masalah</t>
   </si>
@@ -458,6 +458,46 @@
   </si>
   <si>
     <t>Duhhh, baca ulang, cari tahu  dan tambahkan tentang metode, keterkaitan dan pembaruan</t>
+  </si>
+  <si>
+    <t>Metode</t>
+  </si>
+  <si>
+    <t>Keterkaitan Penelitiian</t>
+  </si>
+  <si>
+    <t>Pembaruan</t>
+  </si>
+  <si>
+    <t>IoT-Based Non-Intrusive Automated Driver Drowsiness Monitoring Framework for Logistics and Public Transport Applications to Enhance Road Safety</t>
+  </si>
+  <si>
+    <t>Judul journal penelitian terdahulu</t>
+  </si>
+  <si>
+    <t>Drowsiness Detection Based On Driver Temporal
+Behavior Using a New Developed Dataset</t>
+  </si>
+  <si>
+    <t>Vision Transformers and YoloV5 based Driver Drowsiness Detection Framework</t>
+  </si>
+  <si>
+    <t>Aplikasi Warning Alert Pendeteksi Kelelahan
+Ekspresi Wajah Pada Pengemudi Secara Real-Time
+Menggunakan Metode You Only Look Once
+Berbasis Website</t>
+  </si>
+  <si>
+    <t>Implementasi Algoritma Deep Learning Untuk Sistem Deteksi Kantuk Pada Pengemudi Menggunakan YOLO</t>
+  </si>
+  <si>
+    <t>Driver's Drowsiness Detection System</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Link (Local)</t>
   </si>
 </sst>
 </file>
@@ -467,7 +507,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -487,6 +527,22 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="26"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -512,7 +568,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -563,11 +619,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -641,11 +707,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -653,6 +732,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -688,6 +787,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -718,31 +837,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1391,13 +1500,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E11">
-    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="NOT YET">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="NOT YET">
       <formula>NOT(ISERROR(SEARCH("NOT YET",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="ON PROGRESS">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="ON PROGRESS">
       <formula>NOT(ISERROR(SEARCH("ON PROGRESS",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1413,10 +1522,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D64342-63FD-6945-A4D1-ADCC0106C171}">
-  <dimension ref="B2:F26"/>
+  <dimension ref="B2:N26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,9 +1534,14 @@
     <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="39" customWidth="1"/>
     <col min="6" max="6" width="19.1640625" customWidth="1"/>
+    <col min="9" max="9" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
@@ -1443,8 +1557,29 @@
       <c r="F2" s="7" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="51" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="N2" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="51" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="8">
         <v>1</v>
       </c>
@@ -1460,8 +1595,23 @@
       <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -1477,8 +1627,23 @@
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="J4" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -1494,8 +1659,23 @@
       <c r="F5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="2">
+        <v>3</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -1511,8 +1691,23 @@
       <c r="F6" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H6" s="2">
+        <v>4</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -1528,8 +1723,23 @@
       <c r="F7" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>6</v>
       </c>
@@ -1545,8 +1755,23 @@
       <c r="F8" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="2">
+        <v>6</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>7</v>
       </c>
@@ -1562,8 +1787,14 @@
       <c r="F9" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="28"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>8</v>
       </c>
@@ -1579,8 +1810,14 @@
       <c r="F10" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="28"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>9</v>
       </c>
@@ -1596,8 +1833,14 @@
       <c r="F11" s="3" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="28"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="22">
         <v>10</v>
       </c>
@@ -1613,8 +1856,14 @@
       <c r="F12" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="28"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="22">
         <v>11</v>
       </c>
@@ -1630,8 +1879,14 @@
       <c r="F13" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H13" s="28"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="22">
         <v>12</v>
       </c>
@@ -1647,41 +1902,67 @@
       <c r="F14" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="H14" s="28"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:F14">
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="NOT YET">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="NOT YET">
       <formula>NOT(ISERROR(SEARCH("NOT YET",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="ON PROGRESS">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="ON PROGRESS">
       <formula>NOT(ISERROR(SEARCH("ON PROGRESS",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E14">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="EASY">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="HARD">
+      <formula>NOT(ISERROR(SEARCH("HARD",E3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="EASY">
       <formula>NOT(ISERROR(SEARCH("EASY",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E3)))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N8">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NOT YET">
+      <formula>NOT(ISERROR(SEARCH("NOT YET",N3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="HARD">
-      <formula>NOT(ISERROR(SEARCH("HARD",E3)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="ON PROGRESS">
+      <formula>NOT(ISERROR(SEARCH("ON PROGRESS",N3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",N3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F14" xr:uid="{F3C3F2A3-C474-D04C-91EB-021D5BB25D98}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F14 N3:N8" xr:uid="{F3C3F2A3-C474-D04C-91EB-021D5BB25D98}">
       <formula1>"DONE,ON PROGRESS,NOT YET"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E14" xr:uid="{4AA611BC-D7B5-FF4B-B9D9-783561503493}">
       <formula1>"EASY,MEDIUM,HARD,WHATT????"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{D9BF7A77-65E1-CC48-AB73-B90E6EC52281}"/>
+    <hyperlink ref="J4" r:id="rId2" xr:uid="{5FD61031-992D-9745-A8E0-6AAE4B3F6593}"/>
+    <hyperlink ref="J5:J8" r:id="rId3" display="Link" xr:uid="{5438AFA1-99AB-1041-9DBE-45C8DA837482}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{BA6BB536-99A9-764B-9ACB-04D14B921048}"/>
+    <hyperlink ref="J8" r:id="rId5" xr:uid="{60E25D37-D781-834B-A400-26C0AF89DEEE}"/>
+    <hyperlink ref="J6" r:id="rId6" xr:uid="{DE1D1C7F-F0A9-1D4C-85DC-705405C55129}"/>
+    <hyperlink ref="J7" r:id="rId7" xr:uid="{D76BACA4-66C0-EF4C-8ECF-3D4E02F87614}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
penambahan metode dan pembaruan pada penelitian terdahulu
</commit_message>
<xml_diff>
--- a/docs/skripsi/Progress.xlsx
+++ b/docs/skripsi/Progress.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfauzanzulkarnaen/Documents/Project Skripsi/skripsi-yolov8/docs/skripsi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BB4DEB-4F5E-8E45-8A11-8B01EBB125BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693CD83B-E5F1-974F-8095-2B3FECFFA994}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="20520" activeTab="1" xr2:uid="{A05E2602-9300-1745-9CF0-C349C3E8FD48}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress 1" sheetId="2" r:id="rId1"/>
     <sheet name="Progress 2" sheetId="7" r:id="rId2"/>
-    <sheet name="Note" sheetId="3" r:id="rId3"/>
-    <sheet name="Pytorch" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId3"/>
+    <sheet name="Note" sheetId="3" r:id="rId4"/>
+    <sheet name="Pytorch" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="155">
   <si>
     <t>bab 3 tulis identifikasi masalah</t>
   </si>
@@ -498,6 +499,63 @@
   </si>
   <si>
     <t>Link (Local)</t>
+  </si>
+  <si>
+    <t>Sama sama face detection untuk drowsiness</t>
+  </si>
+  <si>
+    <t>RPL</t>
+  </si>
+  <si>
+    <t>UI UX</t>
+  </si>
+  <si>
+    <t>BIOMEDICAL</t>
+  </si>
+  <si>
+    <t>DATA MINING</t>
+  </si>
+  <si>
+    <t>MULTI MEDIA PROCESSING</t>
+  </si>
+  <si>
+    <t>Komunikasi Visual</t>
+  </si>
+  <si>
+    <t>pelatihan algoritma Haar Cascade untuk pengenalan wajah. Algoritma ini kemudian diterapkan pada aplikasi berbasis Android untuk mendeteksi wajah pengemudi secara otomatis. Sistem ini bertujuan untuk memantau tanda-tanda kelelahan pada pengemudi dalam konteks logistik dan transportasi umum, sehingga dapat meningkatkan keselamatan jalan raya.</t>
+  </si>
+  <si>
+    <t>embaruan dalam penelitian ini meliputi penerapan sistem menggunakan aplikasi Android yang terintegrasi dengan server, memungkinkan pemantauan kondisi pengemudi secara real-time. Integrasi ini bertujuan untuk meningkatkan efektivitas deteksi kelelahan pengemudi pada aplikasi berbasis Android, mendukung pengawasan dan peningkatan keselamatan dalam lalu lantas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> penggunaan algoritma YOLOv3 untuk deteksi objek. Algoritma ini kemudian digabungkan dengan LSTM (Long Short-Term Memory) dalam proses pelatihan data untuk menganalisis perilaku temporal pengemudi. Kombinasi ini bertujuan untuk meningkatkan akurasi deteksi tanda-tanda kelelahan pada pengemudi.</t>
+  </si>
+  <si>
+    <t>peningkatan efektivitas sistem melalui integrasi algoritma YOLOv3 dengan LSTM. LSTM digunakan untuk menganalisis data urutan waktu (temporal data) dari perilaku pengemudi, memungkinkan sistem untuk mendeteksi tanda-tanda kelelahan dengan lebih akurat berdasarkan pola perilaku yang berubah seiring waktu.</t>
+  </si>
+  <si>
+    <t>penerapan YOLOv5 yang dibantu dengan Vision Transformers untuk meningkatkan akurasi klasifikasi. Integrasi Vision Transformers membantu sistem dalam memahami dan menganalisis fitur visual secara lebih mendalam, sehingga meningkatkan kemampuan deteksi kantuk pada pengemudi.</t>
+  </si>
+  <si>
+    <t>penerapan YOLOv5 untuk deteksi objek. Algoritma YOLOv5 kemudian digabungkan dengan Vision Transformers untuk menganalisis dan mengklasifikasikan fitur visual dari wajah dan perilaku pengemudi. Kombinasi ini bertujuan untuk meningkatkan akurasi deteksi tanda-tanda kelelahan pada pengemudi</t>
+  </si>
+  <si>
+    <t>penggunaan website serta bot Telegram untuk membantu mengirimkan informasi kepada pengemudi ataupun pengawas. Integrasi ini memungkinkan pemantauan dan pemberian peringatan secara real-time, sehingga meningkatkan respons terhadap tanda-tanda kelelahan pada pengemudi.</t>
+  </si>
+  <si>
+    <t>pelatihan YOLOv4 dengan dataset RAKIBUL.ECE.RUET. Algoritma YOLOv4 diterapkan untuk mendeteksi ekspresi wajah yang menunjukkan tanda-tanda kelelahan pada pengemudi secara real-time melalui aplikasi berbasis web. Kombinasi ini bertujuan untuk meningkatkan akurasi dan efisiensi deteksi kelelahan pada pengemudi.</t>
+  </si>
+  <si>
+    <t>melakukan uji coba variasi pelatihan untuk memperoleh akurasi maksimal. Dengan menguji berbagai konfigurasi dan parameter pelatihan, penelitian ini bertujuan untuk mengoptimalkan kinerja algoritma YOLOv4 dalam mendeteksi tanda-tanda kantuk pada pengemudi.</t>
+  </si>
+  <si>
+    <t>pelatihan algoritma YOLOv4 menggunakan dataset open source. Algoritma YOLOv4 diterapkan untuk mendeteksi ekspresi wajah yang menunjukkan tanda-tanda kantuk pada pengemudi. Penelitian ini fokus pada pengujian berbagai variasi pelatihan untuk meningkatkan akurasi deteksi kantuk secara keseluruhan.</t>
+  </si>
+  <si>
+    <t>optimalisasi pelatihan menggunakan CUDA dan Adam optimizer untuk memaksimalkan efisiensi pelatihan. Penggunaan CUDA memungkinkan pemrosesan paralel pada GPU, sementara Adam optimizer meningkatkan kecepatan konvergensi dan stabilitas model selama pelatihan.</t>
+  </si>
+  <si>
+    <t>pelatihan YOLOv5 agar dapat melakukan deteksi wajah. Algoritma YOLOv5 diterapkan untuk mendeteksi ekspresi wajah yang menunjukkan tanda-tanda kantuk pada pengemudi. Penelitian ini mengoptimalkan proses pelatihan dengan menggunakan CUDA dan Adam optimizer untuk meningkatkan efisiensi dan akurasi deteksi.</t>
   </si>
 </sst>
 </file>
@@ -724,7 +782,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -812,46 +870,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1524,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D64342-63FD-6945-A4D1-ADCC0106C171}">
   <dimension ref="B2:N26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1604,11 +1622,17 @@
       <c r="J3" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
+      <c r="K3" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="L3" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="M3" s="29" t="s">
+        <v>144</v>
+      </c>
       <c r="N3" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1636,9 +1660,15 @@
       <c r="J4" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
+      <c r="K4" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>146</v>
+      </c>
       <c r="N4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1668,9 +1698,15 @@
       <c r="J5" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
+      <c r="K5" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="L5" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>147</v>
+      </c>
       <c r="N5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1700,9 +1736,15 @@
       <c r="J6" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
+      <c r="K6" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="L6" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>149</v>
+      </c>
       <c r="N6" s="3" t="s">
         <v>1</v>
       </c>
@@ -1732,9 +1774,15 @@
       <c r="J7" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
+      <c r="K7" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="L7" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>151</v>
+      </c>
       <c r="N7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1764,9 +1812,15 @@
       <c r="J8" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
+      <c r="K8" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="L8" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="M8" s="29" t="s">
+        <v>153</v>
+      </c>
       <c r="N8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1968,6 +2022,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC9EC5C-4AE6-C04B-8978-EBE8AF87149A}">
+  <dimension ref="C3:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6442856-5F95-2C47-8D55-0ABD5674E0FC}">
   <dimension ref="B3:E5"/>
   <sheetViews>
@@ -2023,12 +2125,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC091DCD-8BEB-5F43-A16C-3C3A53E95F29}">
   <dimension ref="B2:G192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
@@ -3013,12 +3115,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6752C4-E658-D941-B38E-B79487B40535}">
   <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
rumusan masalah, identifikasi masalah dan bab 4'
</commit_message>
<xml_diff>
--- a/docs/skripsi/Progress.xlsx
+++ b/docs/skripsi/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfauzanzulkarnaen/Documents/Project Skripsi/skripsi-yolov8/docs/skripsi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693CD83B-E5F1-974F-8095-2B3FECFFA994}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFA0922-5A7B-9448-88FB-3BB88A8E325F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="20520" activeTab="1" xr2:uid="{A05E2602-9300-1745-9CF0-C349C3E8FD48}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="157">
   <si>
     <t>bab 3 tulis identifikasi masalah</t>
   </si>
@@ -386,9 +386,6 @@
     <t>Jika menyinggung keakuratan maka harus ada pembanding</t>
   </si>
   <si>
-    <t>Saran permasalahan dijadikan 3 point, dan 1 penekanan 2 nya pendukung</t>
-  </si>
-  <si>
     <t xml:space="preserve">Batasan masalah tidak perlu tertulis alasan, cukup menekankan batasan sesuai area penelitian. </t>
   </si>
   <si>
@@ -453,9 +450,6 @@
   </si>
   <si>
     <t>HARD</t>
-  </si>
-  <si>
-    <t>ON PROGRESS</t>
   </si>
   <si>
     <t>Duhhh, baca ulang, cari tahu  dan tambahkan tentang metode, keterkaitan dan pembaruan</t>
@@ -501,9 +495,6 @@
     <t>Link (Local)</t>
   </si>
   <si>
-    <t>Sama sama face detection untuk drowsiness</t>
-  </si>
-  <si>
     <t>RPL</t>
   </si>
   <si>
@@ -556,6 +547,21 @@
   </si>
   <si>
     <t>pelatihan YOLOv5 agar dapat melakukan deteksi wajah. Algoritma YOLOv5 diterapkan untuk mendeteksi ekspresi wajah yang menunjukkan tanda-tanda kantuk pada pengemudi. Penelitian ini mengoptimalkan proses pelatihan dengan menggunakan CUDA dan Adam optimizer untuk meningkatkan efisiensi dan akurasi deteksi.</t>
+  </si>
+  <si>
+    <t>Melakukan pelatihan dan pengembangan algoritma untuk deteksi lelah pengemudi melalui mimik wajah</t>
+  </si>
+  <si>
+    <t>Menggunakan yolo sebagai algoritma utama untuk melakukan pengembangan teknologi deteksi wajah mengantuk/lelah bagi pengemudi</t>
+  </si>
+  <si>
+    <t>Penerapan yolo untuk pengembangan teknologi deteksi wajah lelah pengemudi</t>
+  </si>
+  <si>
+    <t>permasalahan dijadikan 3 point, dan 1 penekanan 2 nya pendukung</t>
+  </si>
+  <si>
+    <t>Kalau gitu kesimpulan berubah, karena rumusan masalah berubah</t>
   </si>
 </sst>
 </file>
@@ -565,7 +571,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -605,8 +611,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -625,8 +637,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -686,12 +704,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -776,6 +820,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1000,6 +1050,67 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>149000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>620700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCD56F9C-8F2A-A546-B0D4-5772CC844DC6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13081000" y="4038600"/>
+          <a:ext cx="1800000" cy="1573200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -1542,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D64342-63FD-6945-A4D1-ADCC0106C171}">
   <dimension ref="B2:N26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1570,31 +1681,31 @@
         <v>11</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H2" s="27" t="s">
         <v>28</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K2" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="M2" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="L2" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="M2" s="27" t="s">
-        <v>126</v>
-      </c>
       <c r="N2" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="51" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1605,10 +1716,10 @@
         <v>94</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>7</v>
@@ -1617,19 +1728,19 @@
         <v>1</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>7</v>
@@ -1643,10 +1754,10 @@
         <v>95</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>7</v>
@@ -1655,22 +1766,22 @@
         <v>2</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J4" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="L4" s="29" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="M4" s="29" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1681,10 +1792,10 @@
         <v>96</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>7</v>
@@ -1693,22 +1804,22 @@
         <v>3</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J5" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K5" s="29" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L5" s="29" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="M5" s="29" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1719,10 +1830,10 @@
         <v>97</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>1</v>
@@ -1731,22 +1842,22 @@
         <v>4</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J6" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L6" s="29" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="M6" s="29" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1757,10 +1868,10 @@
         <v>98</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>1</v>
@@ -1769,22 +1880,22 @@
         <v>5</v>
       </c>
       <c r="I7" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="J7" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="J7" s="30" t="s">
-        <v>134</v>
-      </c>
       <c r="K7" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L7" s="29" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1792,37 +1903,37 @@
         <v>6</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>99</v>
+        <v>155</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E8" s="26" t="s">
         <v>118</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H8" s="2">
         <v>6</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L8" s="29" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="M8" s="29" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1830,13 +1941,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>7</v>
@@ -1853,13 +1964,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>7</v>
@@ -1876,19 +1987,21 @@
         <v>9</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H11" s="28"/>
-      <c r="I11" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="I11" s="32"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1899,16 +2012,16 @@
         <v>10</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E12" s="26" t="s">
         <v>118</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H12" s="28"/>
       <c r="I12" s="1"/>
@@ -1922,13 +2035,13 @@
         <v>11</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>7</v>
@@ -1945,13 +2058,13 @@
         <v>12</v>
       </c>
       <c r="C14" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="25" t="s">
-        <v>108</v>
-      </c>
       <c r="E14" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>7</v>
@@ -1967,6 +2080,9 @@
       <c r="B26" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H11:I11"/>
+  </mergeCells>
   <conditionalFormatting sqref="F3:F14">
     <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="NOT YET">
       <formula>NOT(ISERROR(SEARCH("NOT YET",F3)))</formula>
@@ -2001,7 +2117,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F14 N3:N8" xr:uid="{F3C3F2A3-C474-D04C-91EB-021D5BB25D98}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N8 F3:F14" xr:uid="{F3C3F2A3-C474-D04C-91EB-021D5BB25D98}">
       <formula1>"DONE,ON PROGRESS,NOT YET"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E14" xr:uid="{4AA611BC-D7B5-FF4B-B9D9-783561503493}">
@@ -2018,6 +2134,7 @@
     <hyperlink ref="J7" r:id="rId7" xr:uid="{D76BACA4-66C0-EF4C-8ECF-3D4E02F87614}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -2036,32 +2153,32 @@
   <sheetData>
     <row r="3" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
benerin label tabel, gambar dan numbering bab dan sub bab
</commit_message>
<xml_diff>
--- a/docs/skripsi/Progress.xlsx
+++ b/docs/skripsi/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfauzanzulkarnaen/Documents/Project Skripsi/skripsi-yolov8/docs/skripsi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFA0922-5A7B-9448-88FB-3BB88A8E325F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE00C225-E0C2-D644-8EA6-B55CFCA3F3CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="20520" activeTab="1" xr2:uid="{A05E2602-9300-1745-9CF0-C349C3E8FD48}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="20520" activeTab="6" xr2:uid="{A05E2602-9300-1745-9CF0-C349C3E8FD48}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress 1" sheetId="2" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="Note" sheetId="3" r:id="rId4"/>
     <sheet name="Pytorch" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="169">
   <si>
     <t>bab 3 tulis identifikasi masalah</t>
   </si>
@@ -562,6 +563,42 @@
   </si>
   <si>
     <t>Kalau gitu kesimpulan berubah, karena rumusan masalah berubah</t>
+  </si>
+  <si>
+    <t>Grafik f1 score di BAB 5</t>
+  </si>
+  <si>
+    <t>Rumusan masalah jadi 2</t>
+  </si>
+  <si>
+    <t>Evaluasi model di Bab 5 Hasil dan pembahasan</t>
+  </si>
+  <si>
+    <t>Garis pembatas kolom di tabel</t>
+  </si>
+  <si>
+    <t>table name size 12</t>
+  </si>
+  <si>
+    <t>gunakan kaidah/symbol yang sesuai dalam flowchart system</t>
+  </si>
+  <si>
+    <t>tambahkan beberapa dataset/foto orang lainnya sebagai pembanding dalam table dan berikan keterangan (kerjakan setelah system selesai saja)</t>
+  </si>
+  <si>
+    <t>Analisa hasil training - ganti gambar table dengan table saja</t>
+  </si>
+  <si>
+    <t>tambahkan installasi dari semua tools yang digunakan</t>
+  </si>
+  <si>
+    <t>buatkan DFD system</t>
+  </si>
+  <si>
+    <t>penulisan (justify/ istilah asing di Italic/ Font dan Size diperhatikan) - nanti sete</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -1653,7 +1690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D64342-63FD-6945-A4D1-ADCC0106C171}">
   <dimension ref="B2:N26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C3" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C3" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -3271,4 +3308,78 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767B0290-C4AA-CD4D-8F5C-2AFDB2D9A5E5}">
+  <dimension ref="A4:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>